<commit_message>
caching enabled and implemented for SpecialtyServiceImpl as well as scheduling of clearing the cache periodically
</commit_message>
<xml_diff>
--- a/src/main/resources/download/Schedule_exampleOF1.xlsx
+++ b/src/main/resources/download/Schedule_exampleOF1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/illia_sitkov/Downloads/university/3 year/fall/spring boot/schedule/src/main/resources/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50037A8-8034-1C4B-B2B3-3F67E0481513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFD99AB-ECD6-F943-A494-2CF5B6861C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="460" windowWidth="13680" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule1" sheetId="1" r:id="rId1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="125" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="132" zoomScaleNormal="179" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>